<commit_message>
change lavamd-rivertrail to use arrays instead of <x,y,z> for positions
</commit_message>
<xml_diff>
--- a/map-reduce/consolidated-numbers.xlsx
+++ b/map-reduce/consolidated-numbers.xlsx
@@ -380,7 +380,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -421,6 +421,10 @@
       <c r="B4">
         <v>148.21251253044201</v>
       </c>
+      <c r="C4">
+        <f>B4/A4</f>
+        <v>11.801264441350257</v>
+      </c>
       <c r="G4">
         <v>18.423354807790801</v>
       </c>
@@ -437,6 +441,10 @@
       </c>
       <c r="B5">
         <v>117.247135544299</v>
+      </c>
+      <c r="C5">
+        <f>B5/A5</f>
+        <v>10.317626018965294</v>
       </c>
       <c r="G5">
         <v>13.796366183377099</v>

</xml_diff>